<commit_message>
Get daily reddit data: Tue Feb 27 08:07:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C437"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2318 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1b15ken</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>ribbons and stars 🎀⭐️</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69r63kcys2lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1b146oo</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Wild flowers</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm5rimste2lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1b13y01</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Mini Nail Tech nails! 🤩</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f5q3uao5c2lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1b13ycm</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Ready for Disney</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b13ycm</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1b12q6a</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Can someone please tell me the difference between types of manicures?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b12q6a/can_someone_please_tell_me_the_difference_between/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1b12l3p</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>CND shades</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b12l3p/cnd_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1b11pk5</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Girly but not.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b11pk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1b10s6r</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>i love the middle finger&lt;3</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1pmdu9pj1lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1b0z8sz</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Nail curving</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0z8sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1b0ytbk</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>My most recent set</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ytbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1b0ylav</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>I made myself shamrock shake nails without realizing it! ☘️</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ylav</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1b0ykmi</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Spring green 🍏</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcedxv2o11lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1b0ygse</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Gel nail broken!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ygse</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1b0xq48</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Matching Valentine's Nails with my boyfriend 💜</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99233iywu0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1b0x8ra</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>There is a gap between my nail and the press on, should I just leave it?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tac0fad7r0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1b0x7m3</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">France </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvgt22lyq0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1b0w4vs</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Cosmic Cliffs</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0w4vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1b0vpad</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Finally did my nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc60el4zf0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1b0vjlj</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">always trying to give the best.!!!!! what do you think? </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aijl999ve0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1b0tzel</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>How to grow back long nail beds?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0tzel/how_to_grow_back_long_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1b0ts5z</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Tips for Polish Application?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0ts5z/tips_for_polish_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1b0uvjj</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>How to keep edges from looking all dry and crusty 😭</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0uvjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1b0um33</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Long black press-on nails that won’t last 3 days?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0um33/long_black_presson_nails_that_wont_last_3_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1b0ud50</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>DND Canadian maple. One of my all time favs</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/447h79hm60lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1b0u0au</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>spring nails! 🌼</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eustrfw540lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1b0tr9r</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>my latest set [1 week of growth]</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0tr9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1b0tc5c</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Photos don’t do this nail foil justice!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orhzoq0jzzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1b0t3xw</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These were fun to make. So many little dots! </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s93sppxxzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1b0t2e3</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I’m currently obsessed with press ons 😍</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cku1esmmxzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1b0sirk</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Legit Qualifications?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0sirk/legit_qualifications/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1b0s4kr</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Just a funny idea</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0s4kr/just_a_funny_idea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1b0rmm6</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle nails 💅 </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euiaf7gpnzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1b0qtrx</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freind of mine did my nails last night, 4 hours but def worth it </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lx9ikey6izkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1b0of56</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Togepi Pokemon inspired nails</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0of56</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1b0q0k0</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>New to gel. Need some pointers!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2so5dw8gczkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1b0pqby</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Recs for gel newbie</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0pqby/recs_for_gel_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1b0pekk</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>jadeite glass nails</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfrzh4368zkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1b0pbls</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>One year progress +fallen ones and the culprit</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0pbls</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1b0p7k1</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tq0jrppr6zkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1b0ok9s</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Recommendations for home builder in a bottle?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0ok9s/recommendations_for_home_builder_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1b0odpt</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Cuticles</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0odpt/cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1b0o9ay</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>What made you start doing your own nails?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0o9ay/what_made_you_start_doing_your_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1b0o5h7</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Got a nail drill for my birthday! So...where do I start? (OG nails done by Corner Salon and Spa</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfm671vbzykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1b0o2kz</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Pink Nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0o2kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1b0nyka</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Did I unknowingly get builder gel??</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0nyka/did_i_unknowingly_get_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1b0nxt8</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I call this one ✨mint toothpaste✨</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4bv0xuvxykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1b0npgu</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvcqry9bwykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1b0crb9</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Nail biter advice. I’ve been a nail biter all my life. Second photo is 4 months of growth and gel nails. First photo is what I did after going back to biting 🥲. I want to fix my nails but I don’t want to wait 4 months again. I’ve never done acyrilics, but are my nails to short for that right now?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0crb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1b0ngjg</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>This set took soo long😭</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ngjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1b0ncdb</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Subtle with GLITTER!</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ncdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1b0bo7b</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Why do my nails grow like this?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxbld55wsvkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1b0naoe</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>New to getting dip nails, what do we think?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0naoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1b0mc1v</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Diving into spring with shades of blue 💙</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3w0o6mpmykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1b0jr05</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Soft skies ☁️</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lq3lsjw3ykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1b0j0v1</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brittle nail treatment </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0j0v1/brittle_nail_treatment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1b0gs16</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Valentine’s Day mismatched theme</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0gs16</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1b0fk97</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with wine red right?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/gregariousdensecreature</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1b0ezmb</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>How to paint Tips without sticking them on your hand first?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ezmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1b0exf7</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying LA Colors Blue/Purple </t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/finy3l0fwwkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1b0eb93</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>New to this, advice needed</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b0eb93/new_to_this_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1b0dpih</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Too cute not to post</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0dpih</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1b0dg92</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>obsessed with doing my own nails⛓️🖤</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7s0teyvewkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1b0dg39</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Some nails for my upcoming Florida trip 😍</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0dg39</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1b0ckju</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Caramel Latte Nails</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koyvxq6v3wkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1b1602d</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Milk glass nails</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kafxmsbsx2lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1b151ft</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Pink hair staining nude nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b151ft/pink_hair_staining_nude_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1b11v13</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Abstract Skittle</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vvtpl4zs1lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1b134zv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Tried Cracked Polish for the first time! (ft all the things I accidentally matched)</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b134zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1b128o1</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Ethereal Pigeon Dupe</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b128o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1b112ju</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Patty Lopes Azureus</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b112ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1b10pkh</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I cried. 6 months of growing my nails out, hard gel supports. Caught my thumb in a window. Don't judge my cuticles, I work a physical job with lots of handwashing! I need a fill but now I have to put it off because my thumb is so damaged :(</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b10pkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1b0zo1q</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Green Glowy Night Butterfly</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0zo1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1b0zm8e</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>How do I make my polish last longer?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0zm8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1b0zcfs</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Does this polish match my skin?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0zcfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1b0ywvy</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>BEE'S KNEES LACQUER Underling (Divine Rivals)</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ywvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1b0yjm1</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Science people, what exactly causes yellowing of the nails? Is it the nitrocellulose in nail polish, or is it highly pigmented colors?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b0yjm1/science_people_what_exactly_causes_yellowing_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1b0yftr</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Marble nails…how do I ask for them at the salon? Nail newbie here!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b0yftr/marble_nailshow_do_i_ask_for_them_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1b0y6fw</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>ILNP - Good Fortune</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0y6fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1b0wsip</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>nail newbie starting a new journey!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0wsip</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1b0wjt6</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Help finding a dupe with just the flakies</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9cxwtq1m0lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1b0w2y6</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>a beautiful sight ☀️</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0w2y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1b0w2t1</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Cosmic Cliffs</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0w2t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1b0vl9g</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>The trouble with nudes</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b0vl9g/the_trouble_with_nudes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1b0vgv0</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I was going for a ✨neutral✨ look</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0vgv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1b0v9jz</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Solo Mission is impressive (swipe for different lighting)</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0v9jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1b0v8uv</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Cuticula Tea Rex</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0v8uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1b0uf1y</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Queen of the Dead Fingertips? I might need to see a doctor about this lol</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3106cbrz60lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1b0thu0</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Another Lyn B banger</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0thu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1b0s62o</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>a little glowy skittle for ya nerves</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t3c9dkkjrzkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1b0s2ko</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>House of Hades may be beautiful but have you seen Sea Glass 😍</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0s2ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1b0r20z</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>West Texas Peyote, alone and with topper</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0r20z</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1b0r03x</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Subtle st paddy mani</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0r03x</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1b0qeuh</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Essie special effects topper in Ethereal Escape over a purple creme (pics 1-3 are in indirect natural light 4-5 are in direct sunlight)</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0qeuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1b0pyoy</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>A Winter-to-Spring Transition Skittle</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqvbluj3czkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1b0pt97</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Sealing the Teal</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/QLprIQn</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1b0ps8q</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Opi scorpio seduction</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ps8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1b0pqbe</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>A bit if sunshine!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0pqbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1b0pgmz</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Mooncat’s Moonicorn 🦄🌕</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0pgmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1b0pden</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Video of the magnetic effect in action!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/06peol3o7zkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1b0pbis</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the wear and tear on a week old mooncat manicure </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdg9pcsj7zkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1b0olyh</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Cygnus Loop - swipe for shift 💙 💜</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0olyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1b0obv6</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Purple skittle in the sun ☀️💜🔮</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0obv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1b0nqyd</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>I don’t use green too often but I love this one! Polishes Used: Cirque Colors (Shade: Introverde) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0nqyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1b0nou0</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>I love the Cirque mxmtoon polishes I got! Polishes Used: Cirque Colors (Shade: Porcelain Plum) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0nou0</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1b0ntm0</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>If Frogs Had Wings</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0ntm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1b0ndvx</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Attempted a Korean blush/jelly nail but my tech didn’t figure it out til the 2nd hand </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnjff6y0uykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1b0n8sk</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>fairy light flicker ✨</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0n8sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1b0n6b8</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Lil Furikake Nails</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0n6b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1b0lyr9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Help a guy make his wife's life easier</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b0lyr9/help_a_guy_make_his_wifes_life_easier/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1b0lj1v</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Decided to get all my polishes out to do a full inventory and reorganization.</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0lj1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1b0l5wt</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>"The Secret of NIMH" -- Lucky 13 Lacquer</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0l5wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1b0kosa</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Haven’t worn black in ages</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oufim6mtaykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1b0k5m9</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Zoya “Hazel”</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcl1qzgx6ykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1b0k318</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>ILNP Velvet Collection swatches (PR - GIFTED)</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0k318</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1b0k047</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Not painting my pinky bright pink is haunting me today. It’s all I can think about when I look at my hands.</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vjnmegt5ykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1b0jmeq</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Indoors v outdoors - plus dog!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0jmeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1b0jax0</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>The magnetic effect is STRONG</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0jax0</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1b0huir</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Experimenting with new color combinations!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj0my9ktoxkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1b0hgu9</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>My favourite colour</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu5ir9qllxkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1b0ev8v</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b0ev8v/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1b0ebqt</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Matchy Matcha</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzoee8eipwkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1b13xaw</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>The cutest bears I made. My client today🧸🧸🧸🧸🧸</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8cv0hj6c2lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1b12xf6</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stilettos in red. </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfgh66zm22lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1b11t2r</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>My nail is made by me.</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b11t2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1b10ruo</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Green freestyle floral set</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b10ruo</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1b0yl4e</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's simple but it makes me happy </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnwt560s11lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1b0whki</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>🐰 pochacco + miffy nails</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0whki</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1b0w2lb</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Hi I just started doing nails few weeks ago so I'm new wanted to ask for yall guys what do u think of these(I'm 16)</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0w2lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1b0scpo</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I just want to know what you guys think of my nails design</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdfpm7osszkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1b0rxhl</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>in love with these set</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3iy01avpzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1b0pvay</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need some help! </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kejpdc5fbzkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1b0pdk4</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[rak_nails_rangeena] Nailart inspired by one of my favourite shows Avatar The Last Air Bender </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6np91ty7zkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1b0nu09</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>When you get lazy with freehand flowers so just add stickers instead 😅</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meocb1r6xykc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1b0mzg7</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Beauty and the beast 🥀</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0mzg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1b0gyk9</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>i can’t get a decent photo of these :( Harry Potter - horcrux nails!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxi69c67hxkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1b0g4ap</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Vacation nails!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egdqdrh89xkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 28 08:07:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C437"/>
+  <dimension ref="A1:C563"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7862,6 +7862,2148 @@
         </is>
       </c>
     </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1b2096v</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Super Cute Nails</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ptvqter3alc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1b207c1</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Healing Nails</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b207c1/healing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1b1y1yv</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Acrylics for DIY 💅</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b1y1yv/acrylics_for_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1b1xwtu</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Do my natural nails look healthy?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1xwtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1b1xlhq</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>French tip gel x- she did my fill in 35 minutes! She did great 🥰</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1xlhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1b1xivf</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do you guys think? </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/did6h5wgb9lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1b1wmuz</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Jumped into the Coquette nails trend 😍💖🎀</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0f5x6ba39lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1b1vn6s</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Two sets of press-ons I made today</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1vn6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1b1qwho</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Nails I did 6 years ago.. I'm still so proud of how I did back then!! ૮ ․ ․ ྀིა🫐💙</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1qwho</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1b1q01g</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>How to stop my nail splitting like this?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m39h83vcl7lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1b1wecl</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>second time doing gel nails on myself:3</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1wecl</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1b1pyvz</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I get acrylics to stay on longer? </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b1pyvz/how_do_i_get_acrylics_to_stay_on_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1b1waq3</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Hard gel over soak off base??</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b1waq3/hard_gel_over_soak_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1b1v5gf</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Gorgeous Press On Nails</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1v5gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1b1treb</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>pink nails &gt;.&lt;</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1treb</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1b1tqw2</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I just found this sub and I love doing nails! Here are some of my past designs</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1tqw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1b1tixd</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>This is not my favourite set that I’ve ever had and there’s some defects (usually my nail tech’s work is practically flawless) but here’s my latest set.</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1tixd</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1b1tfaa</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>So simple, yet so tedious</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1tfaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1b1snox</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this set.  It's giving foggy night vibes </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxhynfxv58lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1b1s0rc</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>How is this shape</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1s0rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1b1rvfj</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Are acrylic nails possible on shorter, natural nails?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b1rvfj/are_acrylic_nails_possible_on_shorter_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1b1qa65</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Never thought brown would look so good on me!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1qa65</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1b1puf2</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Thoughts</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehfv95aak7lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1b1pg5f</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Why did I get bubbles on my polygel?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72xkz8ufh7lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1b1nn88</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>My collection of press on nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuh13wsu47lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1b1p6ma</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>All nails on this hand besides my ring finger broke over the past 2 weeks, so I gave in &amp; am spending time with just nail strengthener (Sally Hansen). Should I be reapplying every other day?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tpy1ookf7lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1b1ncmx</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>So clean ✨</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jtatzes27lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1b1naw5</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>darker aesthetic clawsss</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d46eruag27lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1b1mwyb</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Looking for dupes or listings</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1mwyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1b1kdlp</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Why are they so tilted? Sorry they look bad</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1kdlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1b1jmjb</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Purple Unicorn Inspired Mani 🦄</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1jmjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1b1joke</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>These nails give me life!!!!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ole09v3qc6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1b1jim0</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Which shape</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1jim0</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1b1jgj5</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>just dropping in to show yall my new nails 🌸🐄</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9qddg16b6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1b1ih97</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Mermaid Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1ih97</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1b1923p</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>How can I take care of them after gel?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv54k90xy3lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1b1fiqi</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nails matching my handmade bag 🌻</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcml5rc8j5lc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1b1e4qp</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Stargirl nails</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6pdp8o295lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1b1e3yr</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>My birthday set was gorgeous</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qcb6zvx85lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1b1dpqa</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>New set 😅</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75a76avz55lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1b1dgjh</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Newbie Needs Help</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b1dgjh/newbie_needs_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1b1d6kf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>By me on me!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xhku2ls15lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1b1cdhd</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>I'm just crazy about this polish, it's just crazy😍</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1cdhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1b1cc92</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My new manicure</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1cc92</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1b1bvmp</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>My press on nails i did myself</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52cn4t87r4lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1b1b4gj</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Are these almond nails too pointy?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1b4gj</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1b1axi6</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Zombie Claw Polish - Swamp Puppy</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1axi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1b19av0</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice about pink to white ratio on my nails. </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0oaxhyp14lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1b17qu4</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b17qu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1b1730r</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Sheer black nails with black frame</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1730r</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1b20ayt</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers Crowned Pigeon!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b20ayt</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1b1zzvs</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>had this polish in my cupboard for a while and never used it…until the eras tour!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1zzvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1b1z7v6</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Baths ruined my nails and you saved them</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1z7v6/baths_ruined_my_nails_and_you_saved_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1b1z0yk</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>When you force your family to do ocean themed nails for vacation 🌊✨</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1z0yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1b1z07e</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Poseidon’s prize by mooncat 🌊</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1z07e</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1b1ymkb</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Another crème/jelly/negative space combo</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfcjdgl8m9lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1b1yhzk</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>this month’s nails: february 💕</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1yhzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1b1y7eq</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>How to rehab/heal my proximal nail fold?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1y7eq/how_to_rehabheal_my_proximal_nail_fold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1b1x2ox</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Love how dainty these colors look</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xidwkrqa79lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1b1wz1l</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Essie Berry Naughty</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1wz1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1b1tq0r</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>smoothing base coat for beaus lines ?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1tq0r/smoothing_base_coat_for_beaus_lines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1b1vkjq</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>It's giving Alien Mr. Burns</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1vkjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1b1uqjn</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Ethereal-Pigeon</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/034qdpqwm8lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1b1tob7</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish is different every time I look at my hands! </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iebh2qm7e8lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1b1s7s7</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Mooncat Full Scream Ahead Dandelion puffs</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1s7s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1b1rnpz</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Lights Lacquer 'Ever After' dupe?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8xjeraux7lc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1b1rk6m</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>PPU - Lullaby (Phoenix) and I've Seen Betta Days (Nailed It)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1rk6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1b1pq2s</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Ridge fillers</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1pq2s/ridge_fillers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1b1pa0t</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>new to nails and in need of help!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1pa0t/new_to_nails_and_in_need_of_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1b1oone</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Before (earlier) and after (mani for the week)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1oone</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1b1omle</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Do ILNP collections disappear or do they stay for good?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1omle/do_ilnp_collections_disappear_or_do_they_stay_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1b1o1cr</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>In Bloom</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1o1cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1b1nrus</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>cute girl: compliments me, flirts with me … my silly ass: gets flustered, immediately breaks nail 😩</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1nrus</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1b1nps7</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Clionadh Hippo</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1nps7</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1b1n0ay</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Swatch request</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7q4bz7e07lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1b1makk</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Milk bath with DVN</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1makk</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1b1lh2u</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Little King Trash Mouth 🦝</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1lh2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1b1ld65</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at my nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2gggkhso6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1b1kzr1</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1kzr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1b1kyto</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Blooming Azalea is an instant favorite 🤩</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1kyto</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1b1ku1e</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Orly - Gorgeous 💕</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhbm3qhzk6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1b1kf20</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Yellow and orange jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1kf20</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1b1kdge</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Is this my version of a neutral now?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b24htsoh6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1b1ka3k</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Not What It Seams!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwa3ki01h6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1b1k73z</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Color Club - Midnight Magic</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1k73z</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1b1jx12</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>an unexpected favorite!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1jx12</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1b1jula</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Review Roundup Time! 🩵🌿</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1jula</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1b1jj6v</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Lamp for gels</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1jj6v/lamp_for_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1b1j0bb</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Created this look with 4 kinds of Top Coats, totalling 6 coats on each nail.</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1j0bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1b1izeh</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the extent of my nail art. </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqoh39xo76lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1b1ieau</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Always happens with I wear green</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8r777fi36lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1b1idc0</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Swatch stick advice?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1idc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1b1icv6</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>i used base coat , 3 coats of polish, a top coat , wrapped the edges, dehydrated my nails before application and this sh*t still happens ! HELPPPPPP</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1icv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1b1i0sb</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>This weeks Mani!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1i0sb</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1b1hzyv</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wzd1u8j06lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1b1huth</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>C’est chic vs pele vs wild berry west</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1huth/cest_chic_vs_pele_vs_wild_berry_west/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1b1clc4</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>how to avoid greenies when applying press ons?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1clc4/how_to_avoid_greenies_when_applying_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1b1h20c</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>PPU Skittle ft. no top coat and my winter weary cuticles</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1h20c</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1b1gase</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>First LynB purchase 😍</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rzw7kafso5lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1b1g777</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Thermal nails dedicated to Meryl Streep in Mamma Mia!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1g777</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1b1g23c</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>ILNP Opal Sunset</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1g23c</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1b1fmz3</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Feeling dainty</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1fmz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1b1fj7e</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>How to improve my chrome application?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1fj7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1b1ffkm</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>snubbull nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1ffkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1b1ev78</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>The shift of Phoenix Lullaby</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyxoi9she5lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1b1etz3</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Florals for spring???</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xorujm9e5lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1b1ep43</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>First attempt with nail art</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzlh9zz8d5lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1b1e4hd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Part 2 of the most beautiful color I have ever laid my eyes on </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jvwxi3b195lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1b1e1ii</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wore some fancy matching sweats to run errands and I felt like my nails coordinated really well and it just made me smile. </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fig2mbye85lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1b1dz9w</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Screaming crying rolling on the floor she’s so beautiful</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1dz9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1b1doj9</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Daily Charme Iris topped with Fun Lacquer Shooting Stars</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxe5wfiq55lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1b1bruo</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Aim High</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1bruo</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1b1ayim</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Zombie Claw Polish - Swamp Puppy</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1ayim</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1b1as15</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Best bonding base coat for sensitive nails?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b1as15/best_bonding_base_coat_for_sensitive_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1b16qdx</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here’s a video of the polish from my last post so you guys can see it in it’s true glory </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fsdw79wa63lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1b0xavc</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>First successful stamping session!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b0xavc</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1b20jh5</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>3D Snake Nail Art</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vq4xf777alc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1b1xznz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Tried doing Japanese-style nails!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tr6f3omyf9lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1b1p4dh</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Re-created nail art I saw from this @u/CJgreencheetah user</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjv5wln4f7lc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1b1lgto</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>my natural nails!!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1rdmy6hp6lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1b1iyd2</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Made my first set of press ons and I cannot wait to wear these for spring</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v87u605h76lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1b1dccb</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Floral Print</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1dccb</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1b1cxn3</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Self taught licensed nail technician, here’s my most recent press on sets!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b1cxn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1b1cf4e</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Girly Totoro vibes ✨</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anbyyv8sv4lc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1b17kvd</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Hey everyone it's me again and thank you for all the support I got from the last post:) just made Ocean nail art</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b17kvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1b17kaj</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Very first attempt on myself.</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b17kaj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 29 08:07:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C669"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10004,6 +10004,1808 @@
         </is>
       </c>
     </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1b2rgrc</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>I hit my hand pretty hard yesterday and cracked an acrylic (nail bent backward). My nail underneath is fine, there was no bleeding, but the nail bed is still tender. Should i get my acrylic removed and replaced or will i be fine until my next refill?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2rgrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1b2tlcc</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Strawberry Frenchies</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2tlcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1b2tq7j</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Got My Nails Done Today</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unre83reyglc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1b2t36c</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Structured manicure done with hard gel on my client’s natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2t36c</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1b2suw7</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>ready for spring!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxxqv9lepglc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1b2rx29</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🔥 </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4a6nmjfgglc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1b2rubd</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>recent set 🍃🖤</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2rubd</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1b2rjcd</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Feeling peachy 🍑</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8b2sodrcglc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1b2rff0</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>not bad for an at home job!</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2rff0</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1b2qugd</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Went for the Korean Jelly nail trend, I think my nail tech nailed it.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2qugd</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1b2po95</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Bad edges, but I'm still practicing and my hands are shaky</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2po95</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1b2pmck</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>is the accent ring finger still a thing?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2pmck</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1b2oljf</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Pinky nail broke. Can I put an acrylic set on it or is it too small?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rad6626zmflc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1b2o1ns</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Manicure before or after heavy yard work?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2o1ns/manicure_before_or_after_heavy_yard_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1b2mx0x</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Got acrylics for the first time - not stoked at all about them. I have a dremel, every grit of sandpaper under the sun, and steady hands. Can I clean these suckers up at home?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2mx0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1b2mqzh</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>red cat eye ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3n4t1fl7flc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1b2mqlv</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Tried press ons!!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjxvolli7flc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1b2mgkk</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2mgkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1b2m58l</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>valentines day nails</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv3x9mfv2flc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1b2lu5x</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Got my nails done again 💜💙🕸️</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2lu5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1b2kkst</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Different brand polish and top/base coats? </t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9hwdmn7relc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1b2izwa</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuo9cv39gelc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1b2izop</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Vacay nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdfrmu07gelc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1b2iadp</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Nail Correction</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu942t4abelc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1b2i59a</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic or Gel for growing out nails? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2i59a/acrylic_or_gel_for_growing_out_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1b2i2k5</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Coffee and nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/haybzkcr9elc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1b2ht9x</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Matte leopard French 🔥</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anoz08g08elc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1b2hj2d</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>a few of you asked for side pics bc they looked bulky from the top 😗</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyfp8h616elc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1b2go9u</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Basic♡</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iswwpup30elc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1b2gnm0</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Idk what to ask for at the salon</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2gnm0/idk_what_to_ask_for_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1b2g5en</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Honey’s Nail Course Class- ATL ‘24</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2g5en</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1b2ej9d</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>nail lady popped off!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ej9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1b2ei5b</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>I tried square for the first time, does it suit me? Should I try coffin next? °ʚ(*´꒳`*)ɞ°</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ei5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1b2dfr7</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpeodg7tddlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1b2d6l8</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>New set. What do you think?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql0v4b32cdlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1b2cyys</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2cyys/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1b26guj</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Add zero length but add thickness?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b26guj/add_zero_length_but_add_thickness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1b24s72</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>2nd to last day of Feb, and here are my V-Day inspired nails🙈 inspo pic from @heygreatnails on YT</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b24s72</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1b2byh7</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Feeling Festive with some St. Patty’s Day Nails!🍀</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2byh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1b2bxws</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Gel-x sets lasting for some but not others?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2bxws/gelx_sets_lasting_for_some_but_not_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1b2aiwh</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>BEE HAPPY! Free hand art 🐝</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2aiwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1b2a6l7</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Metallic nails 😃</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38sfotdnrclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1b2a2ot</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>DIY Press On Nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2a2ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1b29wkl</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>it's giving "funky" ✨</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhdjpnttpclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1b299iz</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>New nail tech</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0fx3amblclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1b28wjd</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Help!!! Why am I struggling so much to apply Kokoist color gel?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b28wjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1b28qzv</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Favourite nails I’ve done on myself in 2023</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b28qzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1b28n41</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Shimmery white pedi</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b28n41</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1b26g58</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Gel nails</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b26g58</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1b25tl1</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>I can’t stop staring 😍</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/srg65kiltblc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1b23r8f</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Beachy theme aquarium nails</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h6uahgq39blc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1b22p1e</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I have no idea that difficult nail art is expensive lol and they deserve big tips with this beauty so I have to show off haha</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh4zm039xalc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1b22d0x</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>"Not quite Spring yet" nails</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lztcewibtalc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1b21evq</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>I think I’m in love 💛</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6vwlnbshalc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1b2rn8o</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Turquoise creme with toppers</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/hNaFFEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1b2r6b1</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Question about thermals....</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2r6b1/question_about_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1b2qf5h</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Trying to convince myself I don’t *need* Cadillacquer’s shade for PPU this month</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2qf5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1b2od0o</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Trying to manifest spring through my nail polish choices 💚🌱 Polishes Used: I Scream Nails (Shade: High on Holo) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2od0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1b2qmac</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Matcha Polish Recs</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2qmac</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1b2pezm</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest Reviews Requested :The Manicurist </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2pezm/honest_reviews_requested_the_manicurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1b2ov2f</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Wasn't sure what to expect from Canmake Tokyo, but was pleasantly surprised and delighted with this sheer blue!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ov2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1b2ohqi</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My first go at velvet nails 😁</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwxnv194mflc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1b2o8qn</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Ultimate Neutral Creme Skittle 🤍🤎</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2o8qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1b2ne35</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Added a layer of jade jelly over my mani and love it even more!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5an317sucflc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1b2n0gr</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>My belated Valentine’s Day Mani 💌</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2n0gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1b2mar5</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Shifty Magnetic Sparkles!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqh1jtk04flc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1b2llsy</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Double Bond favorite scents</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2llsy/double_bond_favorite_scents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1b2kj2q</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Phoenix Indie Carina. Think I meant to buy Caraxes, Carina is not exactly red.....</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x459kkuqelc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1b2j0ny</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Bubble bath + birthday girl = new favourite combo!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uv9bxwegelc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1b2imc0</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Thanks to everyone for all the good ideas yesterday about my peeling nails , i appreciate you all so much!🙏🏻💚</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3hhs14kldelc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1b2iapb</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Phoenix “Lullaby” w/ a matte TC</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2iapb</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1b2i7b9</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Best cheap polishes?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2i7b9/best_cheap_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1b2hyb1</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>huzzah</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/paxc04hx8elc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1b2hogg</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>haven’t painted my nails in two weeks but this one got me excited again! ✨</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2hogg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1b2hl12</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Feb mani and reviews</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2hl12</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1b2g39c</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Polished for Days A Winking Light</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2g39c</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1b2fpw2</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>How do you bait a French mermaid? 🍷🧀</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2fpw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1b2f4wp</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Mooncat - Queen of the Dead</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2f4wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1b2ewq9</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>My own Lincoln park after dark</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ewq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1b2eqrd</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>February manis!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2eqrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1b2epao</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Alien Infatuation 💚</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs4blg7imdlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1b2ek20</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Losing my mind staring at the little galaxies on my nails rn</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ek20</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1b2dc4x</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My final “wintry” mani’s</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2dc4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1b2d2ti</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Glowy polish is my dopamine - featuring judgy cat</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2d2ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1b2d05m</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Anyone have this polish? If so, is the shimmer the exact same as in Coffee Cloud? ☕️ ☁️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zwc823tadlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1b2cji5</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Wanting to learn nail art!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2cji5/wanting_to_learn_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1b2cioo</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Emily De Molly - Any good?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2cioo/emily_de_molly_any_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1b2cc9u</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Velvet holo nails courtesy of Cirque Colors’ Black Swan 🖤</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/go4h1u4b6dlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1b2atyj</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>petals for a narcissist in the sun &lt;3</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2atyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1b29qgl</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>ILNP Ball Drop is crazy</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b29qgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1b29g74</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>the collection thus far 🌈 (with &amp; without flash)</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b29g74</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1b28ezb</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you paint over things like builder gel/acrylics? </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b28ezb/can_you_paint_over_things_like_builder_gelacrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1b27wmu</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I’m so excited for Dune Part Two that I had to do some Fremen inspired nails. May thy knife chip and shatter (but not your nails).</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b27wmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1b273x9</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Monarch Lacquers Icicles At Dusk is BEAUTIFUL😭💕</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b273x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1b2rl4c</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Miffy nails!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2rl4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1b2qmwl</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>My perf vday nails by Liv at Mon Amie in Tulsa❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2qmwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1b2oyi0</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>I did my nails today 🦋</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scx08ihzpflc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1b2bk7y</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>What do you think of my skill?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2bk7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1b2acvk</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Question about chrome/hard gel application</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtpv0thxsclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1b2960l</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>what you think about these nails?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/620rfrplkclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1b28lce</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Shimmery white pedi</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b28lce</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1b27uiz</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Feeling Blue 💙</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvh4nj8maclc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1b27fml</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>purple mouse</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9f6msba7clc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1b24ivd</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Blue purple chrome</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bdja239hblc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1b240lw</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Beachy theme aquarium nails</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jvn54yatbblc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1b23q79</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>The nails vs the inspo 💅🏽 My nail tech took inspo from my Red Era dress</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b23q79</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar  1 08:07:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C669"/>
+  <dimension ref="A1:C826"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11806,6 +11806,2675 @@
         </is>
       </c>
     </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1b3oo70</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My Friday nails. Have a great weekend 😘🩷</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vozd28ifolc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1b3nbae</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I think about this old set daily. Such crisp square edges😫</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y88b61h00olc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1b3mvmk</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alice in wonderland set I did! What do you think? </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v0xgmslvnlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1b3mirh</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing Gel Nails on myself </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zxabg90snlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1b3m9ru</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Nails done for the first time in years!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3whz8wnkpnlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1b3lo6v</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Do these look like press on’s I had the salon do it?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3lo6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1b3lhl6</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails came out looking kinda lumpy and chunky? Or is it just me? </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1n1p0l2inlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1b3l3f9</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Too subtle?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ykep6qaenlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1b3ery7</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Is it even worth it?!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3ery7/is_it_even_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1b3ifev</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6x68el4rmlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1b3j6c4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Latex free skin protector?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3j6c4/latex_free_skin_protector/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1b3klhp</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3klhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1b3kaia</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Silver magnetics lookin classy!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3kaia</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1b3k7ie</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I'm in love!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3k7ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1b3k12o</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>First time doing press ons!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3k12o</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1b3jsjg</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Hand painted and they're my real nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obdw6aiq2nlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1b3jrwl</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Strawberry milkshake nails🍓</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afus0hzk2nlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1b3jmwh</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Milky french mani</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycq9g31h1nlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1b3j863</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>I really feel like I struck gold with this combo</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3j863</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1b3ilki</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting Moxie &amp; Millie Nail set from Helluva Boss 💜 she has a 3d tailllll 💕 </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gqkadnfjsmlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1b3hor3</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Made some nails I thought would look good with my opal engagement ring 🥰</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3hor3</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1b3hc12</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Glamnetic nails applied at nail salon professionally - what do you think?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3hc12</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1b3h51l</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Russian manicure I got today!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0yjj0dngmlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1b3g3k8</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Nails for next 3 weeks :D</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q5v5v2d8mlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1b3g24x</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>This design was my idea and my nail tech nailed it 😜</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3g24x</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1b3fu52</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Just thought I’d drop my nail set I did here 🎀</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3fu52</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1b3fjhx</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Cat eye nails on sns</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3fjhx/cat_eye_nails_on_sns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1b3eyhx</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Press on nail advice</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x6k0uxqzllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1b3eqqt</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>learning to stamp drawings with my mother's nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmoff4w5yllc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1b3eblv</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best nail glue for sensitive skin? </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3eblv/best_nail_glue_for_sensitive_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1b3dzuz</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Cuticle oil</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3dzuz/cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1b3dxv0</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>I’ve been loving the bright colors lately!!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sxlglo1gsllc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1b3dkcy</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>soak off yesterday and one nail already broke and one is breaking off😭😭😭</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88ik2lmqpllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1b39f2c</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Need advice: Filed my ridges = breakage! Should I do false nails for temp. strength?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b39f2c/need_advice_filed_my_ridges_breakage_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1b3ddbx</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>1st time getting almond shaped nails and 1st time getting chrome.  I 🩷 almond shape now 😊</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7ojmsvcollc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1b3d8r3</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should this lifting be happening 12 days out from full acrylic set application? </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3uv74efnllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1b3d3q1</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Help! I applied press on nails and I hate them, they are stuck fast</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3d3q1/help_i_applied_press_on_nails_and_i_hate_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1b3d30v</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>I know it's not even March yet, but I'm trying to manifest summer ~</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3d30v</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1b3c2z1</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Alternative to getting my nails done</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3c2z1/alternative_to_getting_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1b3brdu</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Crooked finger</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cygozm75dllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1b3aqas</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>spring 🌸</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4jq8a2y5llc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1b3ao93</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Done with Maniko. What do you think?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3ao93</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1b39x6e</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b39x6e/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1b393vo</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Black french manicure… idk how I feel</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b393vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1b37umm</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Yes I’m obsessed with abstract nails lately😍😍</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0or38yalklc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1b369fh</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>it's been a few days since i did these so they don't look that good now (it's regular polish). this one is by far my favorite set, what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b369fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1b366x3</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I painted my nails for the first time 🥹</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjh2tt8b9klc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1b2zd50</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Help me pick a shape for my next set of press ons 💅🏻</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2zd50</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1b364u0</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Bubbles in gel polish</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z19yt3lv8klc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1b35x97</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Love a good topper</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b35x97</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1b353bl</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>New Gel x Nails</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f3yo8eh1klc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1b351vr</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is builder gel? </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b351vr/what_is_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1b34x4j</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - The Golden Afternoon Collection [gift]</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b34x4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1b34q3s</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Fun nails for holiday</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfxsmrjsyjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1b34k1d</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Which nail shape would suit me better?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b34k1d/which_nail_shape_would_suit_me_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1b3449f</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Aurora Flower Themed Nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3449f</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1b33h8n</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Clear Coat Recommendations NEED</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b33h8n/clear_coat_recommendations_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1b31vpu</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>How to ask for a single nail</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soerb2wkdjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1b31vly</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Last set of February 🩵</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b31vly</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1b31ej3</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Matchy matchyyyyy</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4wn9dju9jlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1b31deu</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Love a good bubble bath mani</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5xuse3l9jlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1b318og</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Tootsies</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b318og/tootsies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1b2zqf0</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>I always hate when i need to change the nail master, but i think they’re good</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2zqf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1b2znn6</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>My first time getting a French mani 😍</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cafhbt3ouilc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1b2zg65</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>First time with cat eye</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byyxweupsilc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1b2zfpz</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nail health while having shellac nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2zfpz/nail_health_while_having_shellac_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1b2zcwu</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>coquette (s)nails ⋅˚₊‧ ୨୧ ‧₊˚ ⋅</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl9aau6vrilc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1b2z98n</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>i think i’ve got builder gel application down 🤍</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wge88izsqilc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1b2yas5</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>No matter how I do my fake nails whenever I apply pressure to my finger tips it feels tight???</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b2yas5/no_matter_how_i_do_my_fake_nails_whenever_i_apply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1b2xs6j</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Mushrooms: nature's little umbrella☂️🍄</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2xs6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1b2vjfu</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2vjfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1b3opij</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Petals For A Narcissist 🌸</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3opij</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1b3nzk2</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Paint it Pretty- Seahorse of course</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3nzk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1b3no91</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>February Mani Round Up</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3no91</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1b3n50n</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Essie Willow by the wind 🍃💅🏼</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qysa09h7ynlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1b3n479</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>First PPU!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3n479</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1b3n1qd</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Mooncat- Marmaid Bait. Loving the glow!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2bp5rlcxnlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1b3lkxs</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cirque Colors Paradox after 6 days of wear</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3lkxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1b3labk</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Cuticula</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3labk/cuticula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1b3l9or</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Toppers to layer with neons</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3l9or/toppers_to_layer_with_neons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1b3l47n</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before &amp; After - praise for nail oil </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6o8fzqienlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1b3hslh</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer PPU Feb '24 | Pigeon</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3hslh</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1b3k5zr</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I’m a sucker for blue shimmer</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1cpl4t1t5nlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1b3k2b2</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Nettle and Briar 😃</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3k2b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1b3k208</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>A (Long and Detailed) Natural Nail Shaping Tutorial</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3k208</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1b3jpd3</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Another Pigeon post</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/534gl7502nlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1b3i34z</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Pigeon under a giant LED 💡🐦</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3i34z</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1b3hxdl</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>There's no hope 😫</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3hxdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1b3hh1i</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Joining the ILNP ranks with a Sweet Pea + Fairy Dust accent. 😍</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3hh1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1b3h3tf</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Is Essie Gel Couture Top Coat 00 or 1098</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3h3tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1b3gzbe</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Now I understand the hype about Mooncat polishes</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zybo8nzdfmlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1b3f6yj</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>my first time with flakies (for real this time, lol)</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3f6yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1b3f5ch</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>First time trying ILNP polishes</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfv3fef51mlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1b3f53h</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>A Sassy (thermal) kinda week</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3f53h</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1b3f0uo</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I need a photochromic polish? </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3f0uo/do_i_need_a_photochromic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1b3erwc</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Never too late for Valentine’s nails, right?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3erwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1b3e1mf</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3e1mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1b3dgys</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I abandoned the thermal when I got home...</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3dgys</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1b3dgt8</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Canmake Foundation Colors</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilihr902pllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1b3dgie</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>mixing polishes is so fun!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3dgie</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1b3czme</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Has anyone tried this color by Cirque Colors?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha8yqx3qlllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1b3cz1q</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Comparison request: Cirque Mood Ring vs Mooncat Drown my Demons please?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3cz1q/comparison_request_cirque_mood_ring_vs_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1b3cxb9</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretending like I have the entire OPI Zodiac collection, instead of just three </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxrx6hn9lllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1b3cw2c</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>First venture into holo/boutique lacquers!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3cw2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1b3cj0y</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Which one would y’all use?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fepno8iillc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1b3c2h5</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Has anyone tried layering ridge filler/blurring base across ONLY their free edge lines to better hide them under sheer polish?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3c2h5/has_anyone_tried_layering_ridge_fillerblurring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1b3c1f8</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Suddenly I’m craving Dr. Pepper…</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3c1f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1b3bti0</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Mooncat - House of Hades</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3bti0</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1b3bpkr</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Calling it “Essence of French Tips” lol</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rsmxqxscllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1b3bjor</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Vampy Skittle ❤️</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3bjor</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1b3amzq</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Palette cleanser NOTD</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a9qahfa5llc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1b3aa83</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>vampires are real but ghosts aren’t? 🧛✅👻❌</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3aa83</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1b39ztx</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Is it even possible for me to grow out my nails?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nzdvlcn0llc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1b39yy4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Does anyone else suddenly hate their nails at certain times of the month?? 😭</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkp5f36h0llc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1b38ovk</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>A little wintery but kind of spring too?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxjfv3iarklc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1b38ngl</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone ever had this happen? </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg1v5ohzqklc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1b37yyp</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Cirque's NSFW jelly over Coquette</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b37yyp/cirques_nsfw_jelly_over_coquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1b37s7m</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Gearing up for Spring</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b37s7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1b3716a</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Trying to convince myself that I don’t need Slumber Party Shag</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3716a</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1b36les</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Recommendations on a magnetic topper lacquer?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b36les/recommendations_on_a_magnetic_topper_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1b36je7</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>peach soft focus blurring vnl base coat by Polished for days! this is Fantastic! from feb ppu ‘24</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b36je7</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1b36h0o</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>RIP</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs2bocmabklc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1b363el</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Hawt Diggity Dawg</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b363el</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1b360t7</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Cirque Colors new collection</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b360t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1b35nrl</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Looking for a Holy Grail Base Coat</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b35nrl/looking_for_a_holy_grail_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1b35cip</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>What a pretty drugstore find</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b35cip</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1b34pi9</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - The Golden Afternoon Collection [gift]</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b34pi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1b34kn1</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I'm eloping today and I did my own nails</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hje7h69oxjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1b347wh</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Space is spooky</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b347wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1b342bh</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>DND gels. Are they bad or am I bad?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxxtmxywtjlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1b33ykc</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Finally found a yellow I love</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9c8ybw4tjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1b32uk1</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>‘Blossom’ for spring</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcwp5djxkjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1b32bgc</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>💙🍋Lemona🍋💙</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b32bgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1b323a0</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Getting back into nails 💅 Sally Hansen On Cloud Shine over Revlon Fashionista</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b323a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1b321ag</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Shout out to the teabag hack.. it really works!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b321ag/shout_out_to_the_teabag_hack_it_really_works/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1b31xx8</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Thursday Holo Mani</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o69qiug2ejlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1b31uz7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Options for top coat shrinkage?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b31uz7/options_for_top_coat_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1b2z38s</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>An unexpected one: Polish Me Silly Peacock Glow on black</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15v896y4pilc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1b2yvto</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Vip </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llsl75m4nilc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1b2ygpq</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Pixie Stick 🤩</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ygpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1b2ycdb</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>…I’m actually so lost on what to even do did they mess it up or is this what the colour is like???😭</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2ycdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1b2xnaq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Recommend your favourite pages for someone wanting to get into simple no-fuss nail art</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b2xnaq/recommend_your_favourite_pages_for_someone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1b3mxn2</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Swirls Inspo vs Result</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3mxn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1b3kaxw</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Silver magnetics looking classy!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3kaxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1b3jtpn</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Valorant Duo set</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3jtpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1b3jrb9</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Black nails. My favorites. For my client today</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oazmb4zf2nlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1b3imgq</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting Moxie &amp; Millie Nail set from Helluva Boss 💜 she has a 3d tailllll 💕 </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1cix6edqsmlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1b3h0wu</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Milky pearl nails with shell fragment accent nails. How's my cuticle work? Feel like this is the first time I'm happy with the cuticles :)</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3h0wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1b3cpuv</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Taken up nail art recently, heres my frankenstein nails or as my partner calls them sally nails</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqk6lxrujllc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1b3ap0w</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>My first ever set (be gentle!) using Beetles gel polish and washi paper</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3cg698p5llc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1b34il3</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>🌊 of Color</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vh7l629xjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1b31wj5</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Juliet’s nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggw5f88rdjlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1b31h8q</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Second time painting my nails. Smeared a lil but I’m pretty happy with it :)</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcrdoyrfajlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1b309y2</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nailart practice </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h35tsfye0jlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1b308jb</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Hologram nailart🦄</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lfl5lyo10jlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1b2y8u6</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Fresh set!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv2b100fgilc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1b2xsu5</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Mushrooms: nature's little umbrella☂️🍄</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b2xsu5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar  2 08:06:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C826"/>
+  <dimension ref="A1:C975"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14475,6 +14475,2539 @@
         </is>
       </c>
     </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1b4hs5z</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>evil eye nails 🧿</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivplmarq9vlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1b4h9ns</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I broke my nail on a door today. Does it need to be cut?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4h9ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1b4h59q</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>regular air dry top coat on bt art box nails?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4h59q/regular_air_dry_top_coat_on_bt_art_box_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1b4h4uf</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Trying to get better at my nail art! Thought I would try some fun colours</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4h4uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1b4gwba</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Traveling with Gel Nail Polish</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4gwba/traveling_with_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1b4gm71</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>These are fire…</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4gm71</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1b4gkbj</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>My first set!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4gkbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1b4a4y5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Sally Hansen insta dri sticky</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4a4y5/sally_hansen_insta_dri_sticky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1b4a202</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Polygel alternatives?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4a202</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1b44w0n</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Press on nail question (double sided nail tape)</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b44w0n/press_on_nail_question_double_sided_nail_tape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1b44occ</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Help! How do I fix this?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uffh7zc39slc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1b40tr3</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Help me heal my dead nails</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b40tr3/help_me_heal_my_dead_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1b3y8d1</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>New Essie cosmic chrome topper</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3y8d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1b4ac5b</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Re-Doing Gel Polish Without Removing Existing Gel Polish?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4ac5b/redoing_gel_polish_without_removing_existing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1b4ffs7</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Did some ACOTAR themed nails today🦇✨⛰️</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqa7vdrululc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1b4ep7w</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>My strawberry nails 💋🍓</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49kals1xeulc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1b4am0n</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Nail stamping plates recs</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4am0n/nail_stamping_plates_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1b4edsv</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>This polish is magical irl💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4edsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1b4d3yy</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>I’m obsessed with the glazed donut trend, I should’ve tried this sooner 😭</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqqe4lyn0ulc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1b4cx6x</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I want beautiful natural nails! Where do I start?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4cx6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1b4cwy7</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Spring vibes</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so2qeaj0ztlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1b4cjyn</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Nail broke off during massage</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efsjwzp1wtlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1b4cb70</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Almost forgot to post my February nails ❤️🫢</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5us8hf1utlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1b4ca86</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I secretly hate short nails 🙃</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2myvr8ftttlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1b4c7ga</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>sweet bunny nails~ ₍ ᐢ.ˬ.ᐢ₎🍫🍓</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4c7ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1b4bsl3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Fav gelx press on brand?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4bsl3/fav_gelx_press_on_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1b4bk4p</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Almond? Not almond?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekwc39apntlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1b41fw5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>got these today - Inspo from u/aejigirl on r/Nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b41fw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1b4av7d</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Any Ghibli fans? 👀 I made a set in the the Japanese woodblock print (Ukiyo-e) style!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn8sls8xhtlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1b49peg</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Really proud of how strong my nails are getting after years of nail extensions (this cat eye is going strong at 3 weeks!)</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b49peg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1b495d1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>These nails in pics 3 and 4 I just dislike so much, I want to cry</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b495d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1b48sev</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Love these</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b48sev</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1b48pd2</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>another day learning how to stamp</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kb0lkgp1tlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1b48hcs</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Simple design on Polygel</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl0w5hi30tlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1b481gi</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Gel-X Manicure</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b481gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1b47i8e</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wine nail’s </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjr72ug6tslc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1b477x2</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Magnetic💙💜💚</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b477x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1b46yc5</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in school to be a nail tech &amp; today I did some Keroppi &amp; My Melody nails! </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0ist4b7pslc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1b46589</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>I’m in my soft girl era I guess</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b46589</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1b46313</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>I love them 🥰</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b46313</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1b461u9</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Got a glitter stuck under my nail, help?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b461u9/got_a_glitter_stuck_under_my_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1b460yd</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I’ve been loving documenting my press on nails journey here, made chrome nails</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jubkcehpislc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1b44xdr</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>From February ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/paixu70yaslc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1b44nsd</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>👽Alien Infatuation 💚🩶 My first Holo Taco!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b44nsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1b44lbn</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>What started as an experiement has turned into the female equivalent of the instability beard</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b44lbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1b44a8f</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I was nervous cause i've always had bad experiences with anything besides a basic manicure, but I feel like such a girlypop with these! I went for a nude pink/lavender ombre with light blue chrome on top 🩷 It feels simple and classy with just a little pizzazz ✨✨</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw0gbsve6slc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1b440mz</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Double sided press on nails stickers colors</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxwde2lj4slc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1b43ruy</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>This rainbow holographic is magical</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43ruy</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1b436g1</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I change my thumb from pink to purple? </t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rm7ynqqyrlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1b42w5p</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Builder gel vs. short nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b42w5p/builder_gel_vs_short_nails_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1b42u39</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>❤️🩷💜🧡</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b42u39</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1b42e55</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it weird to have short nails on the thumbs only? </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b42e55/is_it_weird_to_have_short_nails_on_the_thumbs_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1b426u2</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Swirly Nails!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b426u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1b41y8l</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Man down :(</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b41y8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1b40rl5</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Red nails ❤️</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmcrty2ohrlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1b40at7</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Worked really hard to get my nails to this length! </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16d6q3qderlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1b3zxyg</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>i always liked the way my nails curve :3</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3zxyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1b3zcec</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>i’m not crazy these are bad, right?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3zcec</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1b3z2ra</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Accidentally almost all Sally mani!💚💜</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3z2ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1b3yvks</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Fresh sets</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dhvy0zj4rlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1b3yrel</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Blue pearly nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jewjbjhq3rlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1b3yqw0</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mini UV Light ? </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3yqw0/mini_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1b3yg6e</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>went slightly pointier this time</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmkufeei1rlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1b3xghz</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>ILNP polish</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4x72v9guqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1b3x9us</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Can’t get enough of the magical chrome vibes !!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tb0oi25tqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1b3x40e</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Skittle 🖤🩶🤍</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikxeb6ayrqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1b3wgu2</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kawaii 3D set 🐣 on myself </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1e4chh3nqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1b3w2d9</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Discovering press-ons has been huge for me!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pimk7d55kqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1b3vopx</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Friday nails 💅❤️</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvvazof4hqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1b3tynz</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>She like ? 🤣</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekiq571x2qlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1b3tdeq</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>March Green</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6ybibjexplc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1b3t4st</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New mani, what do y'all think? </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fytyqo42vplc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1b3t06q</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Black and glitter</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3t06q</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1b3syz5</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My favorite purple</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dh7irdftplc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1b3sqei</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Essie- Plant one on me. Absolutely love the color. And by all means yes please do 😆</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6iowrq0rplc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1b3sah5</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>☁️🩷💜💙☁️</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3sah5</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1b3r4xk</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>New to nails; a few days old but I like them enough</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3r4xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1b3q5b1</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Mistborn Metals Nails</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pib09wopxolc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1b3q29f</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Does this colour suit my skin?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3q29f</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1b3q1pl</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>I love Blooming gel! But what would you call this style? Watercolor ombre?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3q1pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1b3phmr</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Tortoiseshell tips</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cg4evosgpolc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1b3paso</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Kiara Sky Gelly Tips Not Adhering</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b3paso/kiara_sky_gelly_tips_not_adhering/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1b4i60k</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Update: IT'S ALIVE!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4i60k</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1b4hgcv</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>What I wore in February</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4hgcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1b4ep1y</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>LynB neutral comparison</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4ep1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1b4ec0u</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Love me some Lyn B</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwy7f7webulc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1b4e8sk</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can the mods set up a monthly HHC megathread too? </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4e8sk/can_the_mods_set_up_a_monthly_hhc_megathread_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1b4e5k8</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Broken 💔</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkktwxou9ulc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1b4dxvw</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Super glowy chunky flake polish?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4dxvw/super_glowy_chunky_flake_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1b4cpxd</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Happy March ₍ᐢ. ̫.ᐢ₎</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4cpxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1b4chhj</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Paradox "Meow!!!" (Feb '24 PPU)</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4chhj/paradox_meow_feb_24_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1b4cdvd</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>New topper from Essie!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4cdvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1b4bnao</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>A comparison you didn’t know you might have needed</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4bnao</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1b49m8w</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>It’s Not a Crime to Feel Joy</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b49m8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1b49l8f</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Do we have any nail technician from india here?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b49l8f/do_we_have_any_nail_technician_from_india_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1b498jj</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Anyone know when BKL mystery shades typically become available for individual purchase?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b498jj/anyone_know_when_bkl_mystery_shades_typically/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1b498dv</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Mooncat - Drown My Demons😍</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b498dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1b48bnh</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Too summery? </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h07agc40zslc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1b48bn3</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>My accent choice really only makes sense in the sun</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b48bn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1b4899d</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Recently learned the best manicure lighting in my house is down in the cellar!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gd384j1jyslc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1b47e47</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>How do you keep the top of your nail polish bottle clean?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b47e47/how_do_you_keep_the_top_of_your_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1b47d74</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Recap Time Again</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b47d74/recap_time_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1b474xp</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>BKL Buzz Bag</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b474xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1b46zdk</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Dream Within a Dream💜💚</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b46zdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1b45t33</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Good quality clear polish for making crellies</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b45t33/good_quality_clear_polish_for_making_crellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1b3ytwi</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Nail Type Question</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3ytwi/nail_type_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1b44m9s</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>👽 Alien Infatuation 💚🩶 My first Holo Taco!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b44m9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1b44dum</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Day 7 using regular polish - little to no chipping!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9i04atv37slc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1b43xo3</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Unfortunately Prickly Pear is a perfect match to my dog’s poo bags</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0iir8csz3slc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1b43rt5</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Girl Dragon meets Vessie de Mer 😍</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43rt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1b43kvx</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Learning how to work with flakies</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43kvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1b43hfk</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Look at all the rainbows 🥹</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43hfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1b43707</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Coziest polish I've ever worn</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43707</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1b432w9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Just feeling amazed by the indie polish community</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b432w9/just_feeling_amazed_by_the_indie_polish_community/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1b42ny1</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Happy March ☘️</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbdo3ltxurlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1b42ibg</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>February manis</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b42ibg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1b42c7l</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Going to the movies today</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b42c7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1b419lu</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Pearl with Pink Shift</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/58VKqQx</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1b40r71</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Emily de Molly Leave a Light On</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8puq4rakhrlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1b406er</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>blue on blue !</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b406er</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1b3zxt3</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Emily de Molly Close-up</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhazooaxbrlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1b3zxqi</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Holo taco: Plumb luck &amp; Fake date</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3zxqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1b3zu0k</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Wrapped up an entire month of pinks and red with this</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3zu0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1b3z8i2</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>New [to me] thermal!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nq72uzyz6rlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1b3yyr1</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Love a color shift!💜💚</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3yyr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1b3yqpm</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Mooncat ✨ </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1mnudal3rlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1b3ynft</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Did anyone buy a Cirque lucky bag this month?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3ynft/did_anyone_buy_a_cirque_lucky_bag_this_month/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1b3yf6y</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Spring nail art</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcghe7fb1rlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1b3y17h</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>🔥Thia Is Fine🔥</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3y17h</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1b3xuk1</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6-day-old manicure </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zhxymp7xqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1b3wzzt</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Skittle 🖤🩶🤍</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b7sfjs4rqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1b3wom2</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Not sure if I like this on me...</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxlkgoqqoqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1b3vb5s</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>I had some fun with colorful blobs.</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqirxc56eqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1b3ujyc</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Holo Taco order finally arrived!!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3ujyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1b3ud30</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Cinderella and the Prugly stepsisters</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3ud30</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1b3u86d</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Which of my recent mani's do y'all like best?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3u86d</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1b3ttqp</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver nails by I Scream Nails (Cashed Out) </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed3z4iuo1qlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1b3rn2m</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b3rn2m/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1b3rjke</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>calling this my “optical illusion mani”</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b3rjke</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1b3qqzm</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Bought a new marble stamping plate, rose quartz is now a lot easier!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umket3ey4plc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1b4d8sh</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Trying new stuff</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4d8sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1b4ckbm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Holographic 💕</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4ckbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1b4c788</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>sweet bunny nails~ ₍ ᐢ.ˬ.ᐢ₎🍫🍓</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4c788</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1b4935i</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>A little spring moment in this gloomy day 🌺</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp2uv0xi4tlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1b47rrn</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My Friend [Me Again]</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b47rrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1b43ndd</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>black flame 🖤</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b43ndd</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1b4258z</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Swirly Nails!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4258z</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1b3wj8j</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>First attempt at doing my own gels, with beetles gel polish and mylee uv lamp</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah3owwzlnqlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1b3usu0</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">'Lost Cherry' using Beetles gel polish and MAC glitter </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhocsnk8aqlc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar  3 08:08:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_03.xlsx
+++ b/data/2024_03_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C975"/>
+  <dimension ref="A1:C1137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17008,6 +17008,2760 @@
         </is>
       </c>
     </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1b5b9i0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Sparkly Nude Polish :)</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5b9i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1b5ajh8</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>new set 🤍🤍</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q63dfi1wd2mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1b598lv</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Marbled Nails for this Month</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ohbahc402mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1b593nj</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Wobbly nails help!!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b593nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1b58szc</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>first try at gel</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcmxk0pxv1mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1b56e0s</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Black micro french</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d2hlxna91mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1b55bhz</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>How do I perfect my shaping</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b55bhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1b543kb</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>How do you find good nail techs???</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b543kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1b5378l</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Birthday nails!! which is your fav?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5378l</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1b58jx9</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>I’ve been growing my nails out for almost a year now!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8clxs3oit1mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1b57lw6</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>New favorite….still figuring out the best shape for myself</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b57lw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1b57gbx</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>I swatched some powders and the look terrible! What did I do wrong?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwkgp1v4j1mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1b576iz</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does it take you forever to take off Aprés Gel Extensions? </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b576iz/does_it_take_you_forever_to_take_off_aprés_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1b56y24</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Last two sets🥰</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b56y24</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1b56s97</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Finally growing my nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xiq1q7xc1mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1b56n7l</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Thoughts on putting gel sparkel polish over metalic powder for a high shine red nails?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b56n7l/thoughts_on_putting_gel_sparkel_polish_over/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1b567sd</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>First time liking them</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52hqa74q71mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1b55asj</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>How do we feel about my new set?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dx60q5mqz0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1b54v1c</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>When you swatch Gel on the plastic sticks, do you use the base coat?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b54v1c/when_you_swatch_gel_on_the_plastic_sticks_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1b54pqm</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>sailor moon bow tie nails I did on myself!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b54pqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1b54o8c</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>First skittle</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cte9t8e5u0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1b53ls0</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>I'm giving birth to my first daughter within the next 2 weeks so wanted some cute pink nails🩷💎</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zttzej9l0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1b53k6r</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Can you apply a base coat or clear UV cured gel coat before applying press ons?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b53k6r/can_you_apply_a_base_coat_or_clear_uv_cured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1b53j9y</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>🔮</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b53j9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1b538x1</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Told my nail tech I wanted brown nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoy3n6fdi0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1b531vd</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Gel-X Extra Short Round</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b531vd/gelx_extra_short_round/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1b52u8h</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Spooky Winter Nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b52u8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1b52rmo</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>So proud I’ve been able to stop biting! Here are a few of my recent DIYs.</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b52rmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1b4yx9s</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Not quite spring mani</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vby26o7ilzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1b4v824</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring nails ! </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2odkwnjitylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1b4up0e</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know of a nail polish shade and name like this colour please? A taupe-y yet nude and sheer all at the same time? Credit: @nailsbyhachi on instagram </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2b7qbhkpylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1b50t7l</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>My first manicure</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b50t7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1b50f4s</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Soooo in love with this 😍💗</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kuk3qqrwzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1b5002n</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>A little purpley-blue chrome moment 🥰</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5702tqntzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1b4zza5</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I tried duck nails 💅</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4zza5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1b4zu8n</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>I don't get my nails done regularly but I treated myself to a French manicure for the first time and really like it</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdk0l4pfszlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1b4z9w3</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>first attempt at gel polish and third attempt at a french tip !</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4z9w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1b4yyuf</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>The way a fresh mani just BOOSTS my mood 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl6g6p7ulzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1b4yw5p</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>St Paddy’s 🍀🇮🇪</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4yw5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1b4ympf</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I'm in LOVE!!! 🦋</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4ympf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1b4y1uf</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Color changing (and glowing) skies ☁️🌅</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4y1uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1b4xrj6</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Recently done, one of my fav</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kodvphalczlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1b4x8hw</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Polygel without efile</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipbf8bmn8zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1b4wv0s</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>My top coat holy grail but why is it so hard to find? I’m going to be so sad when I run out</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siqig7ut5zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1b4wtn5</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Pinks Babies</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyzyx3vj5zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1b4wjyh</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Too much for an interview?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro7aexfi3zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1b4wfi9</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What can I do about this?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4wfi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1b4wba6</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My boss told me "You've been working too hard. Enjoy yourself." So I did. 💅</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/393bukbp1zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1b4vu2t</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>hype this up; i wanted something good for springtime and feel like i just immediately jumped to summer nails 🫠🤪</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mndc573yylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1b4vkld</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Gel removal</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4vkld/gel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1b4v7wh</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>first time painting my nails! 🩷</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4v7wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1b4v3gp</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>New Mani! 🍀</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnbiksygsylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1b4ukl7</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice- swimmer who uses press on nails </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4ukl7/advice_swimmer_who_uses_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1b4ukjb</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Ta-Da</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8r995tmoylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1b4u5y4</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Latest nails</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1mxhh2nlylc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1b4u1z0</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Like totally radical</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zef8qiftkylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1b4tyqi</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New set - irresdicent cat eye</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25k132h4kylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1b4to3k</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Practice practice practice</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqalktxxhylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1b4tmit</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Delicate and elegant </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2c9508mhylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1b4tilq</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>fresh set of nails! 🎀</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp4sfo8sgylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1b4t8rj</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Rubber Ducky, You're The One</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7m9dy7qeylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1b4surw</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Espeon inspired nails 💜💖✨</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs3fxmpobylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1b4stgw</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Perfect nail base recs (biab</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4stgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1b4sn3k</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Second time using builder gel!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4sn3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1b4q1tq</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>How do I correct the shape of my nail plate?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4q1tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1b4h0jh</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Why do my nail oil pens smell??</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4h0jh/why_do_my_nail_oil_pens_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1b4rmui</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>IT BROKE AGAIN</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvei47ag2ylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1b4rmc6</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Sparkly 🌟</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4rmc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1b4r8bp</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Early Spring Vibes 💛</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hokdx5e9zxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1b4qzi6</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>I think this set is cute</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3twyzsbxxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1b4qhuo</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>this took me FOREVER to do on my nails but it's cute</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pquab7zetxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1b4q99d</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Product Recs</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b4q99d/product_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1b4pl5w</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Fresh BIAB😍🐮🌸</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0zwyp6ulxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1b4p34l</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Finally painted my nails and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey6qxzjkhxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1b4ootz</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Pink jelly cat eye on clear dip nails. So hard to catch in a photo!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqo5gn77exlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1b4olsl</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Jumping on the Boolba Bandwagon. Can't get enough</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4olsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1b4o0bh</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>First time getting acrylic nails, I love them but are they too far away from the cuticle?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4o0bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1b4mxv4</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>decided last minute to add the flowers 🌸💖</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2kv9vqexwlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1b4mf2z</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>☕</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swzddkrorwlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1b5b9kk</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>OPI Nature Strong experiences?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b5b9kk/opi_nature_strong_experiences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1b5b91e</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>BKL and Ethereal</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b5b91e/bkl_and_ethereal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1b59o9h</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tonight's color </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hx3m0bjl42mc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1b58je3</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>My last Mani wasn't blue enough 🫣</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b58je3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1b58bf3</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>This ol chestnut</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b58bf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1b561lo</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Matched my nails to my running shoes</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b561lo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1b54s06</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Sheer nail polish recs</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b54s06/sheer_nail_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1b57d2g</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>‘Ard As Nails - Flamingo (PPU Feb ‘24)</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b57d2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1b56tc2</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Tiny Dancer by Cirque Colors is UNREAL!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b56tc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1b55b34</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>You Betta Recognize</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b55b34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1b550qp</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St Patrick nails! </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unta1qw9x0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1b54wpe</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Thanks y’all for your recommendations!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b54wpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1b54l37</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Show me your best jelly !</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lcweuget0mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1b54dch</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>In search of the perfect shimmer opal</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b54dch/in_search_of_the_perfect_shimmer_opal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1b542si</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Bought this thermal from seeing it on a post here, I’m in love</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b542si</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1b5343c</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Dupe for Olive &amp; June - Purple Puka</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpcvojoah0mc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1b52h05</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>After Hours</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix1pbbqbc0mc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1b521aw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Misery is My Favorite Color by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5nbunj7z80mc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1b520nf</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Sweet and Sour Lacquer - Take the Leap (PPU Feb ‘24)</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b520nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1b51r60</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Sweet and Sour, Sassy Sauce, Ethereal, and Night Owl</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b51r60</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1b51nqf</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Your prugliest polish?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0lu4h6660mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1b51eo1</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>ethereal skittle</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b51eo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1b5176r</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>The Glow!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5176r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1b5156n</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Poppies</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5156n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1b4wqzg</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>I’m so ready for spring 🪻 Polishes Used: OPI (Shade: Do You Lilac It?) | Sally Hansen (Shade: Moonlit Top Coat) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4wqzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1b510y3</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m back with yet another thermal… digging the cozy chic vibes </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acd9k7sf10mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1b50vca</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Shimmers!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kymjdbd900mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1b50uzv</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Beautiful glow!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b50uzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1b50to2</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>loving mooncat's pomegranate seeds on this rainy day 🌧️☔️</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b50to2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1b50h6i</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>It took so long for my Buzz Bag (box) to come, that another BKL order came in.</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b50h6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1b509xc</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Marc Jacobs Accent Nail</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoe1xe7pvzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1b4zrrp</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Commemorating my boy before I remove him love u bud</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4zrrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1b4zoki</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>February manicures ✨ the month of holo</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4zoki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1b4zecv</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Nebula cat eye nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tt4dsb2pzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1b4yx5q</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Magic Candy</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo6c3z3hlzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1b4xzdf</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Does regular cuticle cleanup cause more/tougher cuticle growth or am I imaging things?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4xzdf/does_regular_cuticle_cleanup_cause_moretougher/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1b4xemq</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Best "Specialty" Top Coats</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4xemq/best_specialty_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1b4x08l</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Let the greens break free!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4x08l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1b4wmsa</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">obviously had to wear ILNP Sandbar to see Dune 2 </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utf0xob44zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1b4wlo6</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in love! </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i34eshv3zlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1b4wg2s</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>got my Cuticula fix 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4wg2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1b4w3xj</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Gorgeous pink from a pink hating person!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4w3xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1b4w31k</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Found at Ross</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7p3ozfzzylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1b4vzv6</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>midnight disco</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo0mwvkczylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1b4vvej</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often do you paint your nails? </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4vvej/how_often_do_you_paint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1b4vt6y</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>So shifty!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4vt6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1b4vq9q</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was craving something simple and clean ✨ two coats of skinny dip and one coat of good to go topcoat! </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywvr4lobxylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1b4vlnt</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>first time painting my nails! 🩷</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4vlnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1b4veev</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Ulta Exclusive Orly Toppers?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4veev/ulta_exclusive_orly_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1b4v741</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have been using OPI nail envy for a week and my nails are destroyed, help! </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4v741/i_have_been_using_opi_nail_envy_for_a_week_and_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1b4v17x</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Metal Coat - Snailworks</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akdgwf74sylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1b4ur3y</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Baroness X Vessie de Mer</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/flt51zzypylc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1b4unfx</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Best/favorite shimmers?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4unfx/bestfavorite_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1b4ujyb</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>That shimmer, that holo 😍 Wildflower Lacquer “Dark Beauty”</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/99bd1xgioylc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1b4tmfg</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Should have named it How Mesmerizing</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e6zsoiskhylc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1b4tigv</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>June Bug</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4tigv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1b4skgb</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I recently bought Mooncat polishes for the first time. I LOVE them, but two are very thick. Can anyone recommend a good thinner please? </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4skgb/i_recently_bought_mooncat_polishes_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1b4rza6</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Couldn't sleep last night</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a47611w45ylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1b4ruca</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Cat-Bear</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yexo35l24ylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1b4qtgj</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>What is this polish?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4qtgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1b4qrwp</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I think I’m in love with this polish</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euew3h3nvxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1b4qejq</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Pre-cleanup Shiny!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4qejq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1b4pqv1</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Blue Lotus 🪷</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4pqv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1b4piw0</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Black and yellow static</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahoa8oiblxlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1b4n1xc</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>We have the ILNP velvet collection at home. The ILNP velvet collection at home:</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2wfno88kywlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1b4mbbn</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is normal waiting time for Nailland? </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4mbbn/what_is_normal_waiting_time_for_nailland/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1b4kqj9</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Nail tips and tools</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b4kqj9/nail_tips_and_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1b5bkch</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwwm5p4dp2mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1b5aybp</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Café de olla</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5aybp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1b59773</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>St Patrick’s nails</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b59773</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1b58iwb</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Flower Power Nails to welcome in the spring time 🌼</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lr5po39t1mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1b5710y</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>How Can I Do This Nail Design On Gel X or Press Ons?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b5710y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1b5628x</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>GelX Set with some Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxf0yzla61mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1b51xm0</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Pink acrylic nails with silver foil, love them so much!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8tcm08880mc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1b50xhv</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Spring Cloud Nails!!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qq19hxp00mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1b50c58</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Glass Roses</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b50c58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1b4yfw7</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>First time painting cherry blossoms</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfli23awhzlc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1b4vz6h</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>My girl @nailedtothecounter just gave me this set to combat the winter blues</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdj3sqp7zylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1b4tzw5</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>New set - irresdicent cat eye</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5qzulhdkylc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1b4rovi</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ladybird nails using gel polish and acrylic paints </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqezyvnv2ylc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1b4q2da</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Chess nail art made by me♟️</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4q2da</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1b4n011</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Matrix nails 💚🖤</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgbmvxl1ywlc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1b4jl7h</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Brown bear</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b4jl7h</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>